<commit_message>
fix php warning message
</commit_message>
<xml_diff>
--- a/ESI-MS-adducts.xlsx
+++ b/ESI-MS-adducts.xlsx
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2249,7 +2249,7 @@
       <c r="E47" s="4">
         <v>-1.0072760000000001</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="10">
         <f t="shared" ref="G47:G61" si="4">$G$8*D47+E47</f>
         <v>283.43635399999999</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="E48" s="4">
         <v>-1.0072760000000001</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="10">
         <f t="shared" si="4"/>
         <v>425.65816899999999</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="E49">
         <v>-19.01839</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="10">
         <f t="shared" si="4"/>
         <v>834.3125</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="E50" s="4">
         <v>-1.0072760000000001</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50" s="10">
         <f t="shared" si="4"/>
         <v>852.32361399999991</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="E51" s="4">
         <v>20.974665999999999</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="10">
         <f t="shared" si="4"/>
         <v>874.30555599999991</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="E52" s="4">
         <v>34.969402000000002</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="10">
         <f t="shared" si="4"/>
         <v>888.3002919999999</v>
       </c>
@@ -2406,7 +2406,7 @@
       <c r="E53" s="4">
         <v>36.948605999999998</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53" s="10">
         <f t="shared" si="4"/>
         <v>890.27949599999999</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="E54" s="4">
         <v>44.998201000000002</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="10">
         <f t="shared" si="4"/>
         <v>898.32909099999995</v>
       </c>
@@ -2458,7 +2458,7 @@
       <c r="E55" s="4">
         <v>59.013851000000003</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="10">
         <f t="shared" si="4"/>
         <v>912.344741</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="E56" s="4">
         <v>78.918885000000003</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="10">
         <f t="shared" si="4"/>
         <v>932.249775</v>
       </c>
@@ -2510,7 +2510,7 @@
       <c r="E57" s="4">
         <v>112.985586</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="10">
         <f t="shared" si="4"/>
         <v>966.31647599999997</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="E58" s="4">
         <v>-1.0072760000000001</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="10">
         <f t="shared" si="4"/>
         <v>1705.6545039999999</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="E59" s="4">
         <v>44.998201000000002</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="10">
         <f t="shared" si="4"/>
         <v>1751.659981</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="E60" s="4">
         <v>59.013851000000003</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="10">
         <f t="shared" si="4"/>
         <v>1765.6756309999998</v>
       </c>
@@ -2614,7 +2614,7 @@
       <c r="E61" s="4">
         <v>1.0072760000000001</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="10">
         <f t="shared" si="4"/>
         <v>2560.9999459999995</v>
       </c>

</xml_diff>